<commit_message>
RDM-12741: caseManagementLocation is added to CT2 and given access to Staff on CT6 to create the case by super user
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/Access_Control_Definition.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/Access_Control_Definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiranyenigala/Projects/CCD/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D4402E-E1CA-7D47-8F8A-2AE99F2C5FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BC8447-5A2D-954C-BCBD-EE515DC082BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="25960" firstSheet="9" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2503" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2499" uniqueCount="376">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1275,12 +1275,6 @@
   <si>
     <t>CaseLocation</t>
   </si>
-  <si>
-    <t>Public</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
 </sst>
 </file>
 
@@ -2133,7 +2127,7 @@
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="587">
+  <cellXfs count="588">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -3685,6 +3679,9 @@
     </xf>
     <xf numFmtId="0" fontId="71" fillId="21" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="71" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="Explanatory Text" xfId="14" builtinId="53"/>
@@ -13907,7 +13904,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -14236,7 +14233,7 @@
   <dimension ref="A1:CR95"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L9" sqref="J9:L9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -16838,7 +16835,7 @@
   <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -17797,8 +17794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:T293"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView showGridLines="0" topLeftCell="A34" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -18388,10 +18385,11 @@
       <c r="P16" s="54"/>
       <c r="R16" s="56"/>
     </row>
-    <row r="17" spans="1:18" s="555" customFormat="1" ht="20" customHeight="1">
+    <row r="17" spans="1:20" s="587" customFormat="1" ht="20" customHeight="1">
       <c r="A17" s="53">
         <v>42736</v>
       </c>
+      <c r="B17" s="53"/>
       <c r="C17" s="555" t="s">
         <v>321</v>
       </c>
@@ -18401,26 +18399,33 @@
       <c r="E17" s="555" t="s">
         <v>373</v>
       </c>
-      <c r="F17" s="555">
+      <c r="F17" s="560">
         <v>5</v>
       </c>
-      <c r="G17" s="555" t="s">
+      <c r="G17" s="57" t="s">
         <v>268</v>
       </c>
-      <c r="H17" s="555" t="s">
+      <c r="H17" s="57" t="s">
         <v>354</v>
       </c>
       <c r="I17" s="555" t="s">
         <v>374</v>
       </c>
-      <c r="J17" s="555">
+      <c r="J17" s="71">
         <v>1</v>
       </c>
-      <c r="P17" s="555" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" s="72" customFormat="1" ht="20" customHeight="1">
+      <c r="K17" s="72"/>
+      <c r="L17" s="72"/>
+      <c r="M17" s="61"/>
+      <c r="N17" s="72"/>
+      <c r="O17" s="72"/>
+      <c r="P17" s="54"/>
+      <c r="Q17" s="72"/>
+      <c r="R17" s="56"/>
+      <c r="S17" s="72"/>
+      <c r="T17" s="72"/>
+    </row>
+    <row r="18" spans="1:20" s="72" customFormat="1" ht="20" customHeight="1">
       <c r="A18" s="53">
         <v>42736</v>
       </c>
@@ -18451,7 +18456,7 @@
       </c>
       <c r="P18" s="54"/>
     </row>
-    <row r="19" spans="1:18" s="72" customFormat="1" ht="20" customHeight="1">
+    <row r="19" spans="1:20" s="72" customFormat="1" ht="20" customHeight="1">
       <c r="A19" s="53">
         <v>42736</v>
       </c>
@@ -18484,7 +18489,7 @@
       <c r="P19" s="54"/>
       <c r="R19" s="56"/>
     </row>
-    <row r="20" spans="1:18" s="72" customFormat="1" ht="18">
+    <row r="20" spans="1:20" s="72" customFormat="1" ht="18">
       <c r="A20" s="53">
         <v>42736</v>
       </c>
@@ -18517,10 +18522,11 @@
       <c r="P20" s="54"/>
       <c r="R20" s="56"/>
     </row>
-    <row r="21" spans="1:18" s="555" customFormat="1" ht="20" customHeight="1">
+    <row r="21" spans="1:20" s="587" customFormat="1" ht="20" customHeight="1">
       <c r="A21" s="53">
         <v>42736</v>
       </c>
+      <c r="B21" s="53"/>
       <c r="C21" s="555" t="s">
         <v>321</v>
       </c>
@@ -18530,26 +18536,33 @@
       <c r="E21" s="555" t="s">
         <v>373</v>
       </c>
-      <c r="F21" s="555">
+      <c r="F21" s="560">
         <v>5</v>
       </c>
-      <c r="G21" s="555" t="s">
+      <c r="G21" s="57" t="s">
         <v>268</v>
       </c>
-      <c r="H21" s="555" t="s">
+      <c r="H21" s="57" t="s">
         <v>354</v>
       </c>
       <c r="I21" s="555" t="s">
         <v>374</v>
       </c>
-      <c r="J21" s="555">
+      <c r="J21" s="71">
         <v>1</v>
       </c>
-      <c r="P21" s="555" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" s="72" customFormat="1" ht="18">
+      <c r="K21" s="72"/>
+      <c r="L21" s="72"/>
+      <c r="M21" s="61"/>
+      <c r="N21" s="72"/>
+      <c r="O21" s="72"/>
+      <c r="P21" s="54"/>
+      <c r="Q21" s="72"/>
+      <c r="R21" s="56"/>
+      <c r="S21" s="72"/>
+      <c r="T21" s="72"/>
+    </row>
+    <row r="22" spans="1:20" s="72" customFormat="1" ht="18">
       <c r="A22" s="53">
         <v>42736</v>
       </c>
@@ -18582,7 +18595,7 @@
       <c r="P22" s="54"/>
       <c r="R22" s="56"/>
     </row>
-    <row r="23" spans="1:18" s="72" customFormat="1" ht="18">
+    <row r="23" spans="1:20" s="72" customFormat="1" ht="18">
       <c r="A23" s="53">
         <v>42736</v>
       </c>
@@ -18613,7 +18626,7 @@
       </c>
       <c r="P23" s="54"/>
     </row>
-    <row r="24" spans="1:18" s="72" customFormat="1" ht="18">
+    <row r="24" spans="1:20" s="72" customFormat="1" ht="18">
       <c r="A24" s="53">
         <v>42736</v>
       </c>
@@ -18646,7 +18659,7 @@
       <c r="P24" s="54"/>
       <c r="R24" s="56"/>
     </row>
-    <row r="25" spans="1:18" s="72" customFormat="1" ht="18">
+    <row r="25" spans="1:20" s="72" customFormat="1" ht="18">
       <c r="A25" s="53">
         <v>42736</v>
       </c>
@@ -18679,7 +18692,7 @@
       <c r="P25" s="54"/>
       <c r="R25" s="56"/>
     </row>
-    <row r="26" spans="1:18" s="72" customFormat="1" ht="20" customHeight="1">
+    <row r="26" spans="1:20" s="72" customFormat="1" ht="20" customHeight="1">
       <c r="A26" s="53">
         <v>42736</v>
       </c>
@@ -18712,10 +18725,11 @@
       <c r="P26" s="54"/>
       <c r="R26" s="56"/>
     </row>
-    <row r="27" spans="1:18" s="555" customFormat="1" ht="20" customHeight="1">
+    <row r="27" spans="1:20" s="587" customFormat="1" ht="20" customHeight="1">
       <c r="A27" s="53">
         <v>42736</v>
       </c>
+      <c r="B27" s="53"/>
       <c r="C27" s="555" t="s">
         <v>321</v>
       </c>
@@ -18725,26 +18739,33 @@
       <c r="E27" s="555" t="s">
         <v>373</v>
       </c>
-      <c r="F27" s="555">
+      <c r="F27" s="560">
         <v>5</v>
       </c>
-      <c r="G27" s="555" t="s">
+      <c r="G27" s="57" t="s">
         <v>268</v>
       </c>
-      <c r="H27" s="555" t="s">
+      <c r="H27" s="57" t="s">
         <v>354</v>
       </c>
       <c r="I27" s="555" t="s">
         <v>374</v>
       </c>
-      <c r="J27" s="555">
+      <c r="J27" s="71">
         <v>1</v>
       </c>
-      <c r="P27" s="555" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" s="72" customFormat="1" ht="19" customHeight="1">
+      <c r="K27" s="72"/>
+      <c r="L27" s="72"/>
+      <c r="M27" s="61"/>
+      <c r="N27" s="72"/>
+      <c r="O27" s="72"/>
+      <c r="P27" s="54"/>
+      <c r="Q27" s="72"/>
+      <c r="R27" s="56"/>
+      <c r="S27" s="72"/>
+      <c r="T27" s="72"/>
+    </row>
+    <row r="28" spans="1:20" s="72" customFormat="1" ht="19" customHeight="1">
       <c r="A28" s="53">
         <v>42736</v>
       </c>
@@ -18775,7 +18796,7 @@
       </c>
       <c r="P28" s="54"/>
     </row>
-    <row r="29" spans="1:18" s="72" customFormat="1" ht="20" customHeight="1">
+    <row r="29" spans="1:20" s="72" customFormat="1" ht="20" customHeight="1">
       <c r="A29" s="53">
         <v>42736</v>
       </c>
@@ -18808,7 +18829,7 @@
       <c r="P29" s="54"/>
       <c r="R29" s="56"/>
     </row>
-    <row r="30" spans="1:18" s="72" customFormat="1" ht="20" customHeight="1">
+    <row r="30" spans="1:20" s="72" customFormat="1" ht="20" customHeight="1">
       <c r="A30" s="53">
         <v>42736</v>
       </c>
@@ -18841,7 +18862,7 @@
       <c r="P30" s="54"/>
       <c r="R30" s="56"/>
     </row>
-    <row r="31" spans="1:18" s="72" customFormat="1" ht="22" customHeight="1">
+    <row r="31" spans="1:20" s="72" customFormat="1" ht="22" customHeight="1">
       <c r="A31" s="53">
         <v>42736</v>
       </c>
@@ -18874,7 +18895,7 @@
       <c r="P31" s="54"/>
       <c r="R31" s="56"/>
     </row>
-    <row r="32" spans="1:18" s="72" customFormat="1" ht="20" customHeight="1">
+    <row r="32" spans="1:20" s="72" customFormat="1" ht="20" customHeight="1">
       <c r="A32" s="53">
         <v>42736</v>
       </c>
@@ -24478,7 +24499,7 @@
   <dimension ref="A1:H68"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD9"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -29285,8 +29306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:G268"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A39" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -32313,8 +32334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:D15"/>
+    <sheetView topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -32593,8 +32614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:EK80"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -33940,8 +33961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AC80" sqref="AC80"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X52" sqref="X52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -35271,7 +35292,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24:E25"/>
+      <selection activeCell="R46" sqref="R46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -36106,7 +36127,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -36712,7 +36733,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -37040,53 +37061,53 @@
       <c r="O10" s="54"/>
     </row>
     <row r="11" spans="1:15" s="318" customFormat="1" ht="21" customHeight="1">
-      <c r="A11" s="53"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="557" t="s">
-        <v>322</v>
+      <c r="A11" s="59"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="555" t="s">
+        <v>321</v>
       </c>
       <c r="D11" s="555" t="s">
-        <v>331</v>
+        <v>373</v>
       </c>
       <c r="E11" s="555" t="s">
-        <v>332</v>
+        <v>374</v>
       </c>
       <c r="F11" s="102"/>
-      <c r="G11" s="561" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="72"/>
+      <c r="G11" s="555" t="s">
+        <v>375</v>
+      </c>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="75"/>
       <c r="K11" s="558" t="s">
-        <v>333</v>
-      </c>
-      <c r="L11" s="72"/>
-      <c r="M11" s="72"/>
+        <v>75</v>
+      </c>
+      <c r="L11" s="75"/>
+      <c r="M11" s="75"/>
       <c r="N11" s="60"/>
       <c r="O11" s="54"/>
     </row>
     <row r="12" spans="1:15" s="318" customFormat="1" ht="21" customHeight="1">
       <c r="A12" s="53"/>
       <c r="B12" s="53"/>
-      <c r="C12" s="555" t="s">
+      <c r="C12" s="557" t="s">
         <v>322</v>
       </c>
       <c r="D12" s="555" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="E12" s="555" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="F12" s="102"/>
       <c r="G12" s="561" t="s">
         <v>68</v>
       </c>
-      <c r="H12" s="339"/>
-      <c r="I12" s="72"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
       <c r="J12" s="72"/>
       <c r="K12" s="558" t="s">
-        <v>319</v>
+        <v>333</v>
       </c>
       <c r="L12" s="72"/>
       <c r="M12" s="72"/>
@@ -37100,10 +37121,10 @@
         <v>322</v>
       </c>
       <c r="D13" s="555" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E13" s="555" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F13" s="102"/>
       <c r="G13" s="561" t="s">
@@ -37113,7 +37134,7 @@
       <c r="I13" s="72"/>
       <c r="J13" s="72"/>
       <c r="K13" s="558" t="s">
-        <v>75</v>
+        <v>319</v>
       </c>
       <c r="L13" s="72"/>
       <c r="M13" s="72"/>
@@ -37127,10 +37148,10 @@
         <v>322</v>
       </c>
       <c r="D14" s="555" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E14" s="555" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F14" s="102"/>
       <c r="G14" s="561" t="s">
@@ -37140,7 +37161,7 @@
       <c r="I14" s="72"/>
       <c r="J14" s="72"/>
       <c r="K14" s="558" t="s">
-        <v>333</v>
+        <v>75</v>
       </c>
       <c r="L14" s="72"/>
       <c r="M14" s="72"/>
@@ -37150,20 +37171,20 @@
     <row r="15" spans="1:15" s="318" customFormat="1" ht="21" customHeight="1">
       <c r="A15" s="53"/>
       <c r="B15" s="53"/>
-      <c r="C15" s="557" t="s">
-        <v>323</v>
+      <c r="C15" s="555" t="s">
+        <v>322</v>
       </c>
       <c r="D15" s="555" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="E15" s="555" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="F15" s="102"/>
       <c r="G15" s="561" t="s">
         <v>68</v>
       </c>
-      <c r="H15" s="54"/>
+      <c r="H15" s="339"/>
       <c r="I15" s="72"/>
       <c r="J15" s="72"/>
       <c r="K15" s="558" t="s">
@@ -37176,28 +37197,28 @@
     </row>
     <row r="16" spans="1:15" s="318" customFormat="1" ht="21" customHeight="1">
       <c r="A16" s="53"/>
-      <c r="B16" s="111"/>
-      <c r="C16" s="555" t="s">
+      <c r="B16" s="53"/>
+      <c r="C16" s="557" t="s">
         <v>323</v>
       </c>
       <c r="D16" s="555" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="E16" s="555" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="F16" s="102"/>
       <c r="G16" s="561" t="s">
         <v>68</v>
       </c>
-      <c r="H16" s="73"/>
-      <c r="I16" s="112"/>
-      <c r="J16" s="112"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="72"/>
+      <c r="J16" s="72"/>
       <c r="K16" s="558" t="s">
-        <v>319</v>
-      </c>
-      <c r="L16" s="112"/>
-      <c r="M16" s="112"/>
+        <v>333</v>
+      </c>
+      <c r="L16" s="72"/>
+      <c r="M16" s="72"/>
       <c r="N16" s="60"/>
       <c r="O16" s="54"/>
     </row>
@@ -37208,10 +37229,10 @@
         <v>323</v>
       </c>
       <c r="D17" s="555" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E17" s="555" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F17" s="102"/>
       <c r="G17" s="561" t="s">
@@ -37221,24 +37242,24 @@
       <c r="I17" s="112"/>
       <c r="J17" s="112"/>
       <c r="K17" s="558" t="s">
-        <v>75</v>
+        <v>319</v>
       </c>
       <c r="L17" s="112"/>
       <c r="M17" s="112"/>
       <c r="N17" s="60"/>
       <c r="O17" s="54"/>
     </row>
-    <row r="18" spans="1:15" s="322" customFormat="1" ht="21" customHeight="1">
-      <c r="A18" s="59"/>
+    <row r="18" spans="1:15" s="318" customFormat="1" ht="21" customHeight="1">
+      <c r="A18" s="53"/>
       <c r="B18" s="111"/>
       <c r="C18" s="555" t="s">
         <v>323</v>
       </c>
       <c r="D18" s="555" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E18" s="555" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F18" s="102"/>
       <c r="G18" s="561" t="s">
@@ -37248,93 +37269,93 @@
       <c r="I18" s="112"/>
       <c r="J18" s="112"/>
       <c r="K18" s="558" t="s">
-        <v>333</v>
+        <v>75</v>
       </c>
       <c r="L18" s="112"/>
       <c r="M18" s="112"/>
       <c r="N18" s="60"/>
-      <c r="O18" s="60"/>
+      <c r="O18" s="54"/>
     </row>
     <row r="19" spans="1:15" s="322" customFormat="1" ht="21" customHeight="1">
-      <c r="A19" s="53"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="557" t="s">
-        <v>324</v>
+      <c r="A19" s="59"/>
+      <c r="B19" s="111"/>
+      <c r="C19" s="555" t="s">
+        <v>323</v>
       </c>
       <c r="D19" s="555" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="E19" s="555" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="F19" s="102"/>
       <c r="G19" s="561" t="s">
         <v>68</v>
       </c>
-      <c r="H19" s="54"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="72"/>
+      <c r="H19" s="73"/>
+      <c r="I19" s="112"/>
+      <c r="J19" s="112"/>
       <c r="K19" s="558" t="s">
         <v>333</v>
       </c>
-      <c r="L19" s="72"/>
-      <c r="M19" s="72"/>
+      <c r="L19" s="112"/>
+      <c r="M19" s="112"/>
       <c r="N19" s="60"/>
       <c r="O19" s="60"/>
     </row>
     <row r="20" spans="1:15" s="322" customFormat="1" ht="21" customHeight="1">
-      <c r="A20" s="59"/>
-      <c r="B20" s="59"/>
-      <c r="C20" s="555" t="s">
+      <c r="A20" s="53"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="557" t="s">
         <v>324</v>
       </c>
       <c r="D20" s="555" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="E20" s="555" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="F20" s="102"/>
       <c r="G20" s="561" t="s">
         <v>68</v>
       </c>
-      <c r="H20" s="60"/>
+      <c r="H20" s="54"/>
       <c r="I20" s="57"/>
-      <c r="J20" s="75"/>
+      <c r="J20" s="72"/>
       <c r="K20" s="558" t="s">
-        <v>319</v>
-      </c>
-      <c r="L20" s="75"/>
-      <c r="M20" s="75"/>
+        <v>333</v>
+      </c>
+      <c r="L20" s="72"/>
+      <c r="M20" s="72"/>
       <c r="N20" s="60"/>
       <c r="O20" s="60"/>
     </row>
-    <row r="21" spans="1:15" s="318" customFormat="1" ht="21" customHeight="1">
-      <c r="A21" s="53"/>
-      <c r="B21" s="53"/>
+    <row r="21" spans="1:15" s="322" customFormat="1" ht="21" customHeight="1">
+      <c r="A21" s="59"/>
+      <c r="B21" s="59"/>
       <c r="C21" s="555" t="s">
         <v>324</v>
       </c>
       <c r="D21" s="555" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E21" s="555" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F21" s="102"/>
       <c r="G21" s="561" t="s">
         <v>68</v>
       </c>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="72"/>
+      <c r="H21" s="60"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="75"/>
       <c r="K21" s="558" t="s">
-        <v>75</v>
-      </c>
-      <c r="L21" s="72"/>
-      <c r="M21" s="72"/>
+        <v>319</v>
+      </c>
+      <c r="L21" s="75"/>
+      <c r="M21" s="75"/>
       <c r="N21" s="60"/>
-      <c r="O21" s="54"/>
+      <c r="O21" s="60"/>
     </row>
     <row r="22" spans="1:15" s="318" customFormat="1" ht="21" customHeight="1">
       <c r="A22" s="53"/>
@@ -37343,10 +37364,10 @@
         <v>324</v>
       </c>
       <c r="D22" s="555" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E22" s="555" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F22" s="102"/>
       <c r="G22" s="561" t="s">
@@ -37356,7 +37377,7 @@
       <c r="I22" s="54"/>
       <c r="J22" s="72"/>
       <c r="K22" s="558" t="s">
-        <v>333</v>
+        <v>75</v>
       </c>
       <c r="L22" s="72"/>
       <c r="M22" s="72"/>
@@ -37366,14 +37387,14 @@
     <row r="23" spans="1:15" s="318" customFormat="1" ht="21" customHeight="1">
       <c r="A23" s="53"/>
       <c r="B23" s="53"/>
-      <c r="C23" s="557" t="s">
-        <v>325</v>
+      <c r="C23" s="555" t="s">
+        <v>324</v>
       </c>
       <c r="D23" s="555" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="E23" s="555" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="F23" s="102"/>
       <c r="G23" s="561" t="s">
@@ -37393,14 +37414,14 @@
     <row r="24" spans="1:15" s="318" customFormat="1" ht="21" customHeight="1">
       <c r="A24" s="53"/>
       <c r="B24" s="53"/>
-      <c r="C24" s="555" t="s">
+      <c r="C24" s="557" t="s">
         <v>325</v>
       </c>
       <c r="D24" s="555" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="E24" s="555" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="F24" s="102"/>
       <c r="G24" s="561" t="s">
@@ -37410,7 +37431,7 @@
       <c r="I24" s="54"/>
       <c r="J24" s="72"/>
       <c r="K24" s="558" t="s">
-        <v>319</v>
+        <v>333</v>
       </c>
       <c r="L24" s="72"/>
       <c r="M24" s="72"/>
@@ -37419,77 +37440,84 @@
     </row>
     <row r="25" spans="1:15" s="318" customFormat="1" ht="21" customHeight="1">
       <c r="A25" s="53"/>
-      <c r="B25" s="111"/>
+      <c r="B25" s="53"/>
       <c r="C25" s="555" t="s">
         <v>325</v>
       </c>
       <c r="D25" s="555" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E25" s="555" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F25" s="102"/>
       <c r="G25" s="561" t="s">
         <v>68</v>
       </c>
-      <c r="H25" s="73"/>
-      <c r="I25" s="112"/>
-      <c r="J25" s="112"/>
+      <c r="H25" s="54"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="72"/>
       <c r="K25" s="558" t="s">
-        <v>75</v>
-      </c>
-      <c r="L25" s="112"/>
-      <c r="M25" s="112"/>
+        <v>319</v>
+      </c>
+      <c r="L25" s="72"/>
+      <c r="M25" s="72"/>
       <c r="N25" s="60"/>
       <c r="O25" s="54"/>
     </row>
     <row r="26" spans="1:15" s="318" customFormat="1" ht="21" customHeight="1">
       <c r="A26" s="53"/>
-      <c r="B26" s="53"/>
+      <c r="B26" s="111"/>
       <c r="C26" s="555" t="s">
         <v>325</v>
       </c>
       <c r="D26" s="555" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E26" s="555" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F26" s="102"/>
       <c r="G26" s="561" t="s">
         <v>68</v>
       </c>
-      <c r="H26" s="54"/>
-      <c r="I26" s="54"/>
-      <c r="J26" s="72"/>
+      <c r="H26" s="73"/>
+      <c r="I26" s="112"/>
+      <c r="J26" s="112"/>
       <c r="K26" s="558" t="s">
-        <v>333</v>
-      </c>
-      <c r="L26" s="72"/>
-      <c r="M26" s="72"/>
+        <v>75</v>
+      </c>
+      <c r="L26" s="112"/>
+      <c r="M26" s="112"/>
       <c r="N26" s="60"/>
       <c r="O26" s="54"/>
     </row>
-    <row r="27" spans="1:15" s="555" customFormat="1" ht="21" customHeight="1">
+    <row r="27" spans="1:15" s="318" customFormat="1" ht="21" customHeight="1">
+      <c r="A27" s="53"/>
+      <c r="B27" s="53"/>
       <c r="C27" s="555" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="D27" s="555" t="s">
-        <v>373</v>
+        <v>339</v>
       </c>
       <c r="E27" s="555" t="s">
-        <v>374</v>
-      </c>
-      <c r="G27" s="555" t="s">
-        <v>375</v>
-      </c>
-      <c r="K27" s="555" t="s">
-        <v>376</v>
-      </c>
-      <c r="N27" s="555" t="s">
-        <v>377</v>
-      </c>
+        <v>340</v>
+      </c>
+      <c r="F27" s="102"/>
+      <c r="G27" s="561" t="s">
+        <v>68</v>
+      </c>
+      <c r="H27" s="54"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="72"/>
+      <c r="K27" s="558" t="s">
+        <v>333</v>
+      </c>
+      <c r="L27" s="72"/>
+      <c r="M27" s="72"/>
+      <c r="N27" s="60"/>
+      <c r="O27" s="54"/>
     </row>
     <row r="28" spans="1:15" s="318" customFormat="1" ht="21" customHeight="1">
       <c r="A28" s="53"/>
@@ -42106,7 +42134,7 @@
   <dimension ref="A1:T90"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E90" sqref="A4:XFD90"/>
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>
@@ -44191,7 +44219,7 @@
   <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A44" sqref="A39:XFD44"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -44691,7 +44719,7 @@
   <dimension ref="A1:O253"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A253" sqref="A4:XFD253"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -49076,7 +49104,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1"/>

</xml_diff>